<commit_message>
modified:   doc/exceptions.xlsx modified:   pom.xml modified:   src/main/java/pers/zhangzhijun/amp/dto/LogDTO.java new file:   src/main/java/pers/zhangzhijun/amp/service/UrlMap.java modified:   src/main/java/pers/zhangzhijun/amp/service/asset/AssetService.java modified:   src/main/java/pers/zhangzhijun/amp/web/AssetResources.java
</commit_message>
<xml_diff>
--- a/doc/exceptions.xlsx
+++ b/doc/exceptions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="104">
   <si>
     <t>ExceptionCode</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +140,290 @@
   </si>
   <si>
     <t>User has no right.</t>
+  </si>
+  <si>
+    <t>/asset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/protocol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/manufacturer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/projectgroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_ASSETID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_MODEL</t>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_TYPE</t>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_PROTOCOL</t>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_STATUS</t>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_MANUFACTURER</t>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_USERNAME</t>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_USERID</t>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_BY_PROJECTGROUP</t>
+  </si>
+  <si>
+    <t>URL_ASSET_DELETE_BY_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ULR_ASSET_TYPE_LIST_BY_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_TYPE_DELETE_BY_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assettype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assetmanufacturer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assetprotocol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_MANUFACTURER_LIST_BY_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_MANUFACTURER_DELETE_BY_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_PROTOCOL_LIST_BY_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_PROTOCOL_DELETE_BY_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_USER_LIST_BY_ROLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_USER_DELETE_BY_USERID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/asset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/asset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_LIST_ALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_CREATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_UPDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_TYPE_UPDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_TYPE_CREATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_TYPE_LIST_ALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_MANUFACTURER_CREATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_MANUFACTURER_UPDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_MANUFACTURER_LIST_ALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_PROTOCOL_CREATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_PROTOCOL_UPDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_ASSET_PROTOCOL_LIST_ALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_USER_CREATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_USER_UPDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_USER_LIST_ALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_PROJECTGROUP_CREATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_PROJECTGROUP_UPDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_PROJECTGROUP_LIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_PROJECTGROUP_DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL_PROJECTGROUP_LIST_BY_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assetId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -400,11 +684,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:C50" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:C50" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <tableColumns count="3">
-    <tableColumn id="1" name="ExceptionName" dataDxfId="9"/>
-    <tableColumn id="2" name="ExceptionCode" dataDxfId="8"/>
-    <tableColumn id="3" name="ExceptionDesc" dataDxfId="7"/>
+    <tableColumn id="1" name="ExceptionName" dataDxfId="7"/>
+    <tableColumn id="2" name="ExceptionCode" dataDxfId="6"/>
+    <tableColumn id="3" name="ExceptionDesc" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -690,7 +974,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -848,13 +1132,13 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
@@ -862,7 +1146,7 @@
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -873,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -884,7 +1168,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -895,7 +1179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -906,68 +1190,30 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -982,13 +1228,517 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="49.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>